<commit_message>
Update scripts and Baukau input table (new detailed scenario)
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau_final.xlsx
+++ b/inst/extdata/Data_entry/Baukau_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB52E412-5BB4-4461-9E32-FFCC47A6B9CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48704FE8-1D4E-4A82-A29B-62D88B662A68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="19080" windowHeight="6820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="19080" windowHeight="6820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
@@ -1407,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A40E2-2E80-40B7-B15A-A7ACC55EFECA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1511,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE5508C-700E-4B9F-9966-495F6EFAF069}">
   <dimension ref="A1:BA137"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1973,7 +1973,7 @@
         <v>0.9</v>
       </c>
       <c r="G12" s="40">
-        <v>0</v>
+        <v>24675</v>
       </c>
       <c r="H12" s="40">
         <v>0</v>
@@ -2730,7 +2730,7 @@
         <v>0.9</v>
       </c>
       <c r="G31" s="40">
-        <v>0</v>
+        <v>13237</v>
       </c>
       <c r="H31" s="40">
         <v>0</v>
@@ -2804,7 +2804,7 @@
         <v>0.9</v>
       </c>
       <c r="G33" s="40">
-        <v>0</v>
+        <v>10562</v>
       </c>
       <c r="H33" s="40">
         <v>0</v>

</xml_diff>

<commit_message>
New data Sheets for the Assessment
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Baukau_final.xlsx
+++ b/inst/extdata/Data_entry/Baukau_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48704FE8-1D4E-4A82-A29B-62D88B662A68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7F33C8-E357-4A79-821E-127BA0B28511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="19080" windowHeight="6820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="19080" windowHeight="6830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
@@ -1413,10 +1413,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1511,25 +1511,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE5508C-700E-4B9F-9966-495F6EFAF069}">
   <dimension ref="A1:BA137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.08984375" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" customWidth="1"/>
     <col min="10" max="10" width="13.54296875" customWidth="1"/>
-    <col min="11" max="11" width="15.6328125" customWidth="1"/>
-    <col min="12" max="12" width="16.90625" customWidth="1"/>
-    <col min="13" max="53" width="10.90625" style="42"/>
+    <col min="11" max="11" width="15.54296875" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" customWidth="1"/>
+    <col min="13" max="53" width="10.81640625" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1690,7 +1690,7 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="40">
-        <v>0</v>
+        <v>2592</v>
       </c>
       <c r="H5" s="40">
         <v>0</v>
@@ -1731,7 +1731,7 @@
         <v>0.9</v>
       </c>
       <c r="G6" s="40">
-        <v>0</v>
+        <v>6015</v>
       </c>
       <c r="H6" s="40">
         <v>0</v>
@@ -1973,7 +1973,7 @@
         <v>0.9</v>
       </c>
       <c r="G12" s="40">
-        <v>24675</v>
+        <v>0</v>
       </c>
       <c r="H12" s="40">
         <v>0</v>
@@ -2730,7 +2730,7 @@
         <v>0.9</v>
       </c>
       <c r="G31" s="40">
-        <v>13237</v>
+        <v>2651</v>
       </c>
       <c r="H31" s="40">
         <v>0</v>
@@ -2804,7 +2804,7 @@
         <v>0.9</v>
       </c>
       <c r="G33" s="40">
-        <v>10562</v>
+        <v>0</v>
       </c>
       <c r="H33" s="40">
         <v>0</v>
@@ -2978,7 +2978,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>